<commit_message>
updated readme and created fx
</commit_message>
<xml_diff>
--- a/04-summary/Regression_Results_Generation_Detailed.xlsx
+++ b/04-summary/Regression_Results_Generation_Detailed.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="28">
   <si>
     <t>Segment</t>
   </si>
@@ -44,9 +44,6 @@
     <t>0.975]</t>
   </si>
   <si>
-    <t>Boomer</t>
-  </si>
-  <si>
     <t>Gen Z</t>
   </si>
   <si>
@@ -56,19 +53,52 @@
     <t>Millennial</t>
   </si>
   <si>
-    <t>VAR10_WORKFORCE_AI_Increase_Opportunity_Growth</t>
+    <t>VAR02_CG_AI_Training_Opo</t>
+  </si>
+  <si>
+    <t>VAR08_JOB_Enchance_Job_Security</t>
+  </si>
+  <si>
+    <t>VAR21_EXPLAIN_clear_descisions</t>
+  </si>
+  <si>
+    <t>VAR25_FAIRNESS_AI_Treats_All_Fair</t>
+  </si>
+  <si>
+    <t>VAR28_PERSONAL_Enhances_Experience</t>
+  </si>
+  <si>
+    <t>VAR01_CG_Training</t>
+  </si>
+  <si>
+    <t>VAR05_CG_AI_Training_Supported</t>
+  </si>
+  <si>
+    <t>VAR16_ETHICS_AI_Developed_Ethical</t>
+  </si>
+  <si>
+    <t>VAR18_GOV_Strict_AI_rules_Usage</t>
+  </si>
+  <si>
+    <t>VAR29_PERONAL_Improves_CS_quality</t>
+  </si>
+  <si>
+    <t>VAR04_CG_AI_Training_helps_skills</t>
+  </si>
+  <si>
+    <t>VAR06_ED_AI_Training_needed</t>
+  </si>
+  <si>
+    <t>VAR14_SAFETY_AI_Need_Protocols</t>
+  </si>
+  <si>
+    <t>VAR20_ACCOUNTABILITY_AI_access_to_ALL_Skill_levels</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
   <si>
     <t>const</t>
-  </si>
-  <si>
-    <t>VAR07_JOB_Postive_Import</t>
-  </si>
-  <si>
-    <t>VAR08_JOB_Enchance_Job_Security</t>
-  </si>
-  <si>
-    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -435,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,318 +508,521 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.248397723922266</v>
+        <v>0.5127318780494068</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>0.3744547533382699</v>
+        <v>0.3390266996682941</v>
       </c>
       <c r="E2">
-        <v>0.2198869775931448</v>
+        <v>0.1075487508403983</v>
       </c>
       <c r="F2">
-        <v>1.702941926970867</v>
+        <v>3.152307181804537</v>
       </c>
       <c r="G2">
-        <v>0.09827469361816774</v>
+        <v>0.001932371728892524</v>
       </c>
       <c r="H2">
-        <v>-0.07344036311387081</v>
+        <v>0.1266385562516114</v>
       </c>
       <c r="I2">
-        <v>0.8223498697904107</v>
+        <v>0.5514148430849769</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0.2377784670622176</v>
+        <v>0.5127318780494068</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>1.586795384303886</v>
+        <v>0.1436327791203715</v>
       </c>
       <c r="E3">
-        <v>0.6665650515861739</v>
+        <v>0.08676111595666068</v>
       </c>
       <c r="F3">
-        <v>2.380555927029043</v>
+        <v>1.655497137590066</v>
       </c>
       <c r="G3">
-        <v>0.01830815916758921</v>
+        <v>0.09977161008776665</v>
       </c>
       <c r="H3">
-        <v>0.2717021698919955</v>
+        <v>-0.02770377471966612</v>
       </c>
       <c r="I3">
-        <v>2.901888598715777</v>
+        <v>0.3149693329604092</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>0.2377784670622176</v>
+        <v>0.5127318780494068</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>0.1685080738461561</v>
+        <v>-0.2737160824347269</v>
       </c>
       <c r="E4">
-        <v>0.09936556569981282</v>
+        <v>0.1157671832971082</v>
       </c>
       <c r="F4">
-        <v>1.695839727368185</v>
+        <v>-2.364366780283962</v>
       </c>
       <c r="G4">
-        <v>0.09160754432316318</v>
+        <v>0.01925312850932138</v>
       </c>
       <c r="H4">
-        <v>-0.02753427924011131</v>
+        <v>-0.5023340527683799</v>
       </c>
       <c r="I4">
-        <v>0.3645504269324235</v>
+        <v>-0.0450981121010739</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.2377784670622176</v>
+        <v>0.5127318780494068</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>0.21442951014188</v>
+        <v>0.1596597412845681</v>
       </c>
       <c r="E5">
-        <v>0.09327803205812514</v>
+        <v>0.07567250779807679</v>
       </c>
       <c r="F5">
-        <v>2.298821120156787</v>
+        <v>2.10987776050189</v>
       </c>
       <c r="G5">
-        <v>0.02263882469440539</v>
+        <v>0.03641491074200761</v>
       </c>
       <c r="H5">
-        <v>0.03039749898043609</v>
+        <v>0.01022106056229125</v>
       </c>
       <c r="I5">
-        <v>0.3984615213033239</v>
+        <v>0.3090984220068449</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>0.2377784670622176</v>
+        <v>0.5127318780494068</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>0.2570546397773372</v>
+        <v>0.1791437701745188</v>
       </c>
       <c r="E6">
-        <v>0.08063760831661829</v>
+        <v>0.1047896211542082</v>
       </c>
       <c r="F6">
-        <v>3.187776090382405</v>
+        <v>1.709556425544197</v>
       </c>
       <c r="G6">
-        <v>0.001684978497929407</v>
+        <v>0.08927455574667599</v>
       </c>
       <c r="H6">
-        <v>0.09796143308844904</v>
+        <v>-0.0277956216117021</v>
       </c>
       <c r="I6">
-        <v>0.4161478464662253</v>
+        <v>0.3860831619607397</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>0.1770417438442555</v>
+        <v>0.4480473588297689</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>1.566996189934805</v>
+        <v>0.1500432733070636</v>
       </c>
       <c r="E7">
-        <v>0.549260741189643</v>
+        <v>0.05346217589225771</v>
       </c>
       <c r="F7">
-        <v>2.852918609367293</v>
+        <v>2.806531361713481</v>
       </c>
       <c r="G7">
-        <v>0.00462713377835058</v>
+        <v>0.005355470734364154</v>
       </c>
       <c r="H7">
-        <v>0.4861901583730424</v>
+        <v>0.04480929269340737</v>
       </c>
       <c r="I7">
-        <v>2.647802221496567</v>
+        <v>0.2552772539207199</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>0.1770417438442555</v>
+        <v>0.4480473588297689</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>0.1727790367024856</v>
+        <v>0.2541010533342766</v>
       </c>
       <c r="E8">
-        <v>0.08410133100571612</v>
+        <v>0.09669595080206445</v>
       </c>
       <c r="F8">
-        <v>2.054415009088766</v>
+        <v>2.627835511482985</v>
       </c>
       <c r="G8">
-        <v>0.04078458911759352</v>
+        <v>0.009061856573959347</v>
       </c>
       <c r="H8">
-        <v>0.007288916989075744</v>
+        <v>0.06376649170643353</v>
       </c>
       <c r="I8">
-        <v>0.3382691564158955</v>
+        <v>0.4444356149621196</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>0.1770417438442555</v>
+        <v>0.4480473588297689</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>0.2722528288093782</v>
+        <v>0.2446740654722274</v>
       </c>
       <c r="E9">
-        <v>0.08839093720513486</v>
+        <v>0.06902456313275801</v>
       </c>
       <c r="F9">
-        <v>3.080098904003502</v>
+        <v>3.5447390663181</v>
       </c>
       <c r="G9">
-        <v>0.00225715390569872</v>
+        <v>0.0004596582549427455</v>
       </c>
       <c r="H9">
-        <v>0.09832185049151959</v>
+        <v>0.1088073631289232</v>
       </c>
       <c r="I9">
-        <v>0.4461838071272369</v>
+        <v>0.3805407678155315</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>0.208757174520633</v>
+        <v>0.4480473588297689</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>1.863533250563887</v>
+        <v>-0.1884648441412313</v>
       </c>
       <c r="E10">
-        <v>0.4653478371262896</v>
+        <v>0.0953617784219976</v>
       </c>
       <c r="F10">
-        <v>4.004602797924142</v>
+        <v>-1.976314276640599</v>
       </c>
       <c r="G10">
-        <v>7.728364068884429E-05</v>
+        <v>0.04909005844791531</v>
       </c>
       <c r="H10">
-        <v>0.9480056012788846</v>
+        <v>-0.3761732449734086</v>
       </c>
       <c r="I10">
-        <v>2.77906089984889</v>
+        <v>-0.0007564433090539169</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.208757174520633</v>
+        <v>0.4480473588297689</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D11">
-        <v>0.3221819470839722</v>
+        <v>-0.1870399973309894</v>
       </c>
       <c r="E11">
-        <v>0.08319159652155991</v>
+        <v>0.09590667644413693</v>
       </c>
       <c r="F11">
-        <v>3.872770334446888</v>
+        <v>-1.950229163033662</v>
       </c>
       <c r="G11">
-        <v>0.0001304911302162323</v>
+        <v>0.05213595176731064</v>
       </c>
       <c r="H11">
-        <v>0.1585103863134423</v>
+        <v>-0.3758209655800596</v>
       </c>
       <c r="I11">
-        <v>0.4858535078545021</v>
+        <v>0.001740970918080814</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.4480473588297689</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>0.3620637462116975</v>
+      </c>
+      <c r="E12">
+        <v>0.08574207230049682</v>
+      </c>
+      <c r="F12">
+        <v>4.222708134960713</v>
+      </c>
+      <c r="G12">
+        <v>3.256902485278988E-05</v>
+      </c>
+      <c r="H12">
+        <v>0.1932906010178094</v>
+      </c>
+      <c r="I12">
+        <v>0.5308368914055857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>0.208757174520633</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>0.1906903711370238</v>
-      </c>
-      <c r="E12">
-        <v>0.07354053113106018</v>
-      </c>
-      <c r="F12">
-        <v>2.592996925697819</v>
-      </c>
-      <c r="G12">
-        <v>0.009951263531097199</v>
-      </c>
-      <c r="H12">
-        <v>0.04600636441772749</v>
-      </c>
-      <c r="I12">
-        <v>0.3353743778563201</v>
+      <c r="D13">
+        <v>0.2057490930311686</v>
+      </c>
+      <c r="E13">
+        <v>0.08771855499302059</v>
+      </c>
+      <c r="F13">
+        <v>2.345559534667885</v>
+      </c>
+      <c r="G13">
+        <v>0.01965636737255073</v>
+      </c>
+      <c r="H13">
+        <v>0.03312042193512441</v>
+      </c>
+      <c r="I13">
+        <v>0.3783777641272129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>0.2032412004226422</v>
+      </c>
+      <c r="E14">
+        <v>0.08547472669503554</v>
+      </c>
+      <c r="F14">
+        <v>2.37779292524426</v>
+      </c>
+      <c r="G14">
+        <v>0.01804937331425542</v>
+      </c>
+      <c r="H14">
+        <v>0.03502834645080477</v>
+      </c>
+      <c r="I14">
+        <v>0.3714540543944796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>0.2558036344552468</v>
+      </c>
+      <c r="E15">
+        <v>0.0711236646026346</v>
+      </c>
+      <c r="F15">
+        <v>3.596603688581187</v>
+      </c>
+      <c r="G15">
+        <v>0.0003774671373178866</v>
+      </c>
+      <c r="H15">
+        <v>0.115833434252901</v>
+      </c>
+      <c r="I15">
+        <v>0.3957738346575926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>0.1582712178028612</v>
+      </c>
+      <c r="E16">
+        <v>0.0864479700128107</v>
+      </c>
+      <c r="F16">
+        <v>1.830826308349485</v>
+      </c>
+      <c r="G16">
+        <v>0.06812829353225205</v>
+      </c>
+      <c r="H16">
+        <v>-0.01185696298453992</v>
+      </c>
+      <c r="I16">
+        <v>0.3283993985902623</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>-0.1556433487622506</v>
+      </c>
+      <c r="E17">
+        <v>0.08332015841979176</v>
+      </c>
+      <c r="F17">
+        <v>-1.868015516462092</v>
+      </c>
+      <c r="G17">
+        <v>0.06274450667102988</v>
+      </c>
+      <c r="H17">
+        <v>-0.3196160478641107</v>
+      </c>
+      <c r="I17">
+        <v>0.008329350339609465</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>0.1512129747882545</v>
+      </c>
+      <c r="E18">
+        <v>0.06529448290932004</v>
+      </c>
+      <c r="F18">
+        <v>2.315861433472975</v>
+      </c>
+      <c r="G18">
+        <v>0.0212467602747658</v>
+      </c>
+      <c r="H18">
+        <v>0.02271450812477457</v>
+      </c>
+      <c r="I18">
+        <v>0.2797114414517345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>0.4295545399991504</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>0.1288298817671446</v>
+      </c>
+      <c r="E19">
+        <v>0.07485905719919204</v>
+      </c>
+      <c r="F19">
+        <v>1.720965860207695</v>
+      </c>
+      <c r="G19">
+        <v>0.08629844287663549</v>
+      </c>
+      <c r="H19">
+        <v>-0.01849150952603734</v>
+      </c>
+      <c r="I19">
+        <v>0.2761512730603266</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +1032,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -839,118 +1072,437 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>0.196339972860453</v>
+        <v>0.3941744380813387</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D2">
-        <v>1.801520282227503</v>
+        <v>0.4459057420051479</v>
       </c>
       <c r="E2">
-        <v>0.133629424591406</v>
+        <v>0.2829449714413738</v>
       </c>
       <c r="F2">
-        <v>13.48146403934573</v>
+        <v>1.575945102447384</v>
       </c>
       <c r="G2">
-        <v>9.655937952813969E-38</v>
+        <v>0.1154083681030108</v>
       </c>
       <c r="H2">
-        <v>1.539244862447435</v>
+        <v>-0.1094423604621592</v>
       </c>
       <c r="I2">
-        <v>2.063795702007571</v>
+        <v>1.001253844472455</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>0.196339972860453</v>
+        <v>0.3941744380813387</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>0.2207355309394138</v>
+        <v>-0.06609158552015006</v>
       </c>
       <c r="E3">
-        <v>0.04690350775433649</v>
+        <v>0.04636110979137431</v>
       </c>
       <c r="F3">
-        <v>4.706162534698816</v>
+        <v>-1.425582472411967</v>
       </c>
       <c r="G3">
-        <v>2.937598827671416E-06</v>
+        <v>0.1543538653010002</v>
       </c>
       <c r="H3">
-        <v>0.1286776834777445</v>
+        <v>-0.1570865030822489</v>
       </c>
       <c r="I3">
-        <v>0.3127933784010831</v>
+        <v>0.02490333204194878</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>0.196339972860453</v>
+        <v>0.3941744380813387</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>0.1643704013803194</v>
+        <v>-0.08159750209940173</v>
       </c>
       <c r="E4">
-        <v>0.04496674321688599</v>
+        <v>0.04520740012418865</v>
       </c>
       <c r="F4">
-        <v>3.655377054716178</v>
+        <v>-1.804958964135215</v>
       </c>
       <c r="G4">
-        <v>0.0002722740487561949</v>
+        <v>0.07143281422742423</v>
       </c>
       <c r="H4">
-        <v>0.07611385541813774</v>
+        <v>-0.1703279847390284</v>
       </c>
       <c r="I4">
-        <v>0.252626947342501</v>
+        <v>0.007132980540224917</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>0.1788555091577344</v>
+      </c>
+      <c r="E5">
+        <v>0.05337673658472489</v>
+      </c>
+      <c r="F5">
+        <v>3.350813867645075</v>
+      </c>
+      <c r="G5">
+        <v>0.0008410622025027039</v>
+      </c>
+      <c r="H5">
+        <v>0.07409072317401803</v>
+      </c>
+      <c r="I5">
+        <v>0.2836202951414507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>-0.0337198578291704</v>
+      </c>
+      <c r="E6">
+        <v>0.04964819605976071</v>
+      </c>
+      <c r="F6">
+        <v>-0.6791758916795761</v>
+      </c>
+      <c r="G6">
+        <v>0.4972102310390955</v>
+      </c>
+      <c r="H6">
+        <v>-0.1311664791006351</v>
+      </c>
+      <c r="I6">
+        <v>0.06372676344229428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
-        <v>0.196339972860453</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D7">
+        <v>0.0661046828209484</v>
+      </c>
+      <c r="E7">
+        <v>0.03046167829390627</v>
+      </c>
+      <c r="F7">
+        <v>2.170093262201261</v>
+      </c>
+      <c r="G7">
+        <v>0.03027447522682052</v>
+      </c>
+      <c r="H7">
+        <v>0.006316254165323491</v>
+      </c>
+      <c r="I7">
+        <v>0.1258931114765733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>0.2017458171445331</v>
-      </c>
-      <c r="E5">
-        <v>0.0423721511676227</v>
-      </c>
-      <c r="F5">
-        <v>4.761283333159884</v>
-      </c>
-      <c r="G5">
-        <v>2.254115095007436E-06</v>
-      </c>
-      <c r="H5">
-        <v>0.1185816954067264</v>
-      </c>
-      <c r="I5">
-        <v>0.2849099388823398</v>
+      <c r="D8">
+        <v>0.03976949103318937</v>
+      </c>
+      <c r="E8">
+        <v>0.03807317323976183</v>
+      </c>
+      <c r="F8">
+        <v>1.044554147949401</v>
+      </c>
+      <c r="G8">
+        <v>0.2965243104111231</v>
+      </c>
+      <c r="H8">
+        <v>-0.03495834175316498</v>
+      </c>
+      <c r="I8">
+        <v>0.1144973238195437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>-0.04715925555178279</v>
+      </c>
+      <c r="E9">
+        <v>0.03422702037977998</v>
+      </c>
+      <c r="F9">
+        <v>-1.377837013812709</v>
+      </c>
+      <c r="G9">
+        <v>0.1686141190712649</v>
+      </c>
+      <c r="H9">
+        <v>-0.1143380809049632</v>
+      </c>
+      <c r="I9">
+        <v>0.0200195698013976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>0.2224696064078709</v>
+      </c>
+      <c r="E10">
+        <v>0.03852855316222113</v>
+      </c>
+      <c r="F10">
+        <v>5.774148992078211</v>
+      </c>
+      <c r="G10">
+        <v>1.081980139144418E-08</v>
+      </c>
+      <c r="H10">
+        <v>0.1468479801232572</v>
+      </c>
+      <c r="I10">
+        <v>0.2980912326924846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>0.2470678032345297</v>
+      </c>
+      <c r="E11">
+        <v>0.04996654946521396</v>
+      </c>
+      <c r="F11">
+        <v>4.944664097858808</v>
+      </c>
+      <c r="G11">
+        <v>9.181320599192628E-07</v>
+      </c>
+      <c r="H11">
+        <v>0.1489963362245744</v>
+      </c>
+      <c r="I11">
+        <v>0.3451392702444849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>0.05595838973950319</v>
+      </c>
+      <c r="E12">
+        <v>0.04510851419412374</v>
+      </c>
+      <c r="F12">
+        <v>1.240528329057508</v>
+      </c>
+      <c r="G12">
+        <v>0.2151203424212206</v>
+      </c>
+      <c r="H12">
+        <v>-0.03257800528887343</v>
+      </c>
+      <c r="I12">
+        <v>0.1444947847678798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>0.2402619357297829</v>
+      </c>
+      <c r="E13">
+        <v>0.04368276327449111</v>
+      </c>
+      <c r="F13">
+        <v>5.500154242075746</v>
+      </c>
+      <c r="G13">
+        <v>5.013700937094167E-08</v>
+      </c>
+      <c r="H13">
+        <v>0.1545239225343666</v>
+      </c>
+      <c r="I13">
+        <v>0.3259999489251992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>-0.101588798513662</v>
+      </c>
+      <c r="E14">
+        <v>0.0402513580769672</v>
+      </c>
+      <c r="F14">
+        <v>-2.523860147014358</v>
+      </c>
+      <c r="G14">
+        <v>0.01178752265142091</v>
+      </c>
+      <c r="H14">
+        <v>-0.1805918471131933</v>
+      </c>
+      <c r="I14">
+        <v>-0.02258574991413073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>0.1125809034540475</v>
+      </c>
+      <c r="E15">
+        <v>0.04846132177850875</v>
+      </c>
+      <c r="F15">
+        <v>2.323108394950423</v>
+      </c>
+      <c r="G15">
+        <v>0.02040711934795946</v>
+      </c>
+      <c r="H15">
+        <v>0.01746381070045254</v>
+      </c>
+      <c r="I15">
+        <v>0.2076979962076424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>0.3941744380813387</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>0.05827951504007783</v>
+      </c>
+      <c r="E16">
+        <v>0.03841531873889955</v>
+      </c>
+      <c r="F16">
+        <v>1.517090498095066</v>
+      </c>
+      <c r="G16">
+        <v>0.1296134697789283</v>
+      </c>
+      <c r="H16">
+        <v>-0.01711986123668002</v>
+      </c>
+      <c r="I16">
+        <v>0.1336788913168357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>